<commit_message>
PDs in data file, updated results
</commit_message>
<xml_diff>
--- a/Biogeme_Logit_Models/Location_Choice/ClosestDummies/Results.xlsx
+++ b/Biogeme_Logit_Models/Location_Choice/ClosestDummies/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\Biogeme_Logit_Models\Location_Choice\ClosestDummies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67746FC-9C95-4409-9EF1-2650E18BC5DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872ADCC8-B003-45B7-ACED-3D612E083F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{EEEC793F-2898-4B2C-A71E-FA7EE3304475}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ASC_SG</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>B_CLOSEST_RY</t>
+  </si>
+  <si>
+    <t>Hardmax Acc</t>
+  </si>
+  <si>
+    <t>Softmax APO</t>
   </si>
 </sst>
 </file>
@@ -133,9 +139,24 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -160,24 +181,166 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -489,413 +652,566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F87847A-CDF4-40AF-B0D1-EFCE09B4A56A}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="12" width="11.7265625" customWidth="1"/>
     <col min="13" max="19" width="13.90625" customWidth="1"/>
+    <col min="20" max="20" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="T1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="21">
         <v>-0.134157802673147</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="22">
         <v>6.5943866412797703E-2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="21">
         <v>0.92020530707048598</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="24">
+        <v>0.49590000000000001</v>
+      </c>
+      <c r="U2" s="25">
+        <v>0.3679</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>-0.12669264665190799</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>6.4885003800214197E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>0.91541091850134204</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2">
         <v>0.33777707323400502</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="16">
+        <v>0.49530000000000002</v>
+      </c>
+      <c r="U3" s="17">
+        <v>0.37159999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>-0.12401769290605399</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>6.5351350998246793E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>0.91417546721111798</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="2">
         <v>0.29066522151021101</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="16">
+        <v>0.49590000000000001</v>
+      </c>
+      <c r="U4" s="17">
+        <v>0.37119999999999997</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>-0.120855039362552</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="8">
         <v>6.5198161020527404E-2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="7">
         <v>0.92910127515623098</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="7">
         <v>0.28322084286315602</v>
       </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="18">
+        <v>0.50350000000000006</v>
+      </c>
+      <c r="U5" s="19">
+        <v>0.37090000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>-0.13582354761641199</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>7.0772400442581193E-2</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2">
+      <c r="D6" s="2"/>
+      <c r="E6" s="5">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="4">
         <v>0.201180231465279</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="4">
         <v>0.23743216871064499</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="4">
         <v>0.207970225515344</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="4">
         <v>6.3575834371409803E-2</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="4">
         <v>0.36184031191094101</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="3">
         <v>6.4706868185952601E-2</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="16">
+        <v>0.49439999999999995</v>
+      </c>
+      <c r="U6" s="17">
+        <v>0.36979999999999996</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>-0.12386949533274</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <v>6.8346785973522006E-2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2">
+      <c r="D7" s="2"/>
+      <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="4">
         <v>-0.18839829787868401</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="4">
         <v>0.33975305355146201</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="4">
         <v>0.30375315839224898</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="4">
         <v>0.18875813947200401</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="4">
         <v>0.47740998325675499</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <v>0.18976757620437101</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
+      <c r="L7" s="2"/>
+      <c r="M7" s="4">
         <v>0.59945514607207295</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="4">
         <v>0.81085719701271597</v>
       </c>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="16">
+        <v>0.50080000000000002</v>
+      </c>
+      <c r="U7" s="17">
+        <v>0.37439999999999996</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>-0.12524508285775399</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <v>6.8314192801803203E-2</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="5">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="4">
         <v>-0.18165802238348799</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="4">
         <v>0.36838298095704097</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="4">
         <v>0.233604940475274</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="4">
         <v>0.146186633154265</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="4">
         <v>0.47375551327934901</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="3">
         <v>0.190044835983841</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1">
+      <c r="L8" s="2"/>
+      <c r="M8" s="4">
         <v>0.59746801572549102</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="4">
         <v>0.788130446745405</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="4">
         <v>-0.102296597267937</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="4">
         <v>0.30420238032853802</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="4">
         <v>0.27039163206589301</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="16">
+        <v>0.50029999999999997</v>
+      </c>
+      <c r="U8" s="17">
+        <v>0.374</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>-0.12537912798571799</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="8">
         <v>6.8494116149463699E-2</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2">
+      <c r="D9" s="7"/>
+      <c r="E9" s="9">
         <v>0</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="10">
         <v>-0.179179657857267</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="10">
         <v>0.37132435452010898</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="10">
         <v>0.23594440868720201</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="10">
         <v>0.14698458909582199</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="10">
         <v>0.47105373921295701</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="8">
         <v>0.20060674810412801</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1">
+      <c r="L9" s="7"/>
+      <c r="M9" s="10">
         <v>0.60371111816346301</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="10">
         <v>0.78920350542210704</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="10">
         <v>-0.102110887772339</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="10">
         <v>0.30488613910259799</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="10">
         <v>0.27318083486495198</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="10">
         <v>1.16030877159158E-2</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="8">
         <v>-5.44786947784658E-2</v>
       </c>
+      <c r="T9" s="18">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="U9" s="19">
+        <v>0.37409999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6:K9">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7:S9">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T2:T9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U2:U9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor format changes for Results
</commit_message>
<xml_diff>
--- a/Biogeme_Logit_Models/Location_Choice/ClosestDummies/Results.xlsx
+++ b/Biogeme_Logit_Models/Location_Choice/ClosestDummies/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\Biogeme_Logit_Models\Location_Choice\ClosestDummies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872ADCC8-B003-45B7-ACED-3D612E083F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F7937A-28DC-4AF5-BEBE-752753E4ACC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{EEEC793F-2898-4B2C-A71E-FA7EE3304475}"/>
   </bookViews>
@@ -266,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -336,6 +336,12 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -654,9 +660,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F87847A-CDF4-40AF-B0D1-EFCE09B4A56A}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R27" sqref="R27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -889,7 +895,9 @@
       <c r="C6" s="3">
         <v>7.0772400442581193E-2</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="26">
+        <v>1</v>
+      </c>
       <c r="E6" s="5">
         <v>0</v>
       </c>
@@ -936,7 +944,9 @@
       <c r="C7" s="3">
         <v>6.8346785973522006E-2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
       <c r="E7" s="5">
         <v>0</v>
       </c>
@@ -987,7 +997,9 @@
       <c r="C8" s="3">
         <v>6.8314192801803203E-2</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="26">
+        <v>1</v>
+      </c>
       <c r="E8" s="5">
         <v>0</v>
       </c>
@@ -1044,7 +1056,9 @@
       <c r="C9" s="8">
         <v>6.8494116149463699E-2</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="27">
+        <v>1</v>
+      </c>
       <c r="E9" s="9">
         <v>0</v>
       </c>
@@ -1152,32 +1166,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:K9">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L3:L5">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M7:S9">
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>